<commit_message>
📊 Horarios actualizados Línea 141 - 1312
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:36:47</t>
+          <t>Última actualización: 02:49:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -478,12 +478,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:36:47</t>
+          <t>02:49:39</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:59</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,23 +503,73 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:36:47</t>
+          <t>02:49:39</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:01</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>02:49:39</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>04:01</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>72</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>02:49:39</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>116</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -536,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,14 +604,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:36:47</t>
+          <t>Última actualización: 02:49:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -595,12 +645,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:36:47</t>
+          <t>02:49:39</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:59</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -609,9 +659,34 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>02:49:39</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>116</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -646,7 +721,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:36:47</t>
+          <t>Última actualización: 02:49:39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1313
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:49:39</t>
+          <t>Última actualización: 03:45:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:49:39</t>
+          <t>03:45:24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>03:46</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:49:39</t>
+          <t>03:45:24</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:49:39</t>
+          <t>03:45:24</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,23 +553,123 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02:49:39</t>
+          <t>03:45:24</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>03:45:24</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>05:16</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>91</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>03:45:24</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>97</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>03:45:24</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>109</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>03:45:24</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05:36</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>111</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -604,7 +704,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:49:39</t>
+          <t>Última actualización: 03:45:24</t>
         </is>
       </c>
     </row>
@@ -645,21 +745,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:49:39</t>
+          <t>03:45:24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -670,21 +770,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:49:39</t>
+          <t>03:45:24</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>05:34</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -703,7 +803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,14 +821,66 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:49:39</t>
+          <t>Última actualización: 03:45:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 0</t>
+          <t>Total filas: 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>03:45:24</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>05:44</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>119</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1314
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:45:24</t>
+          <t>Última actualización: 04:38:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -528,12 +528,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03:45:24</t>
+          <t>04:38:41</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:45</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -558,16 +558,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:45:24</t>
+          <t>04:38:41</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03:45:24</t>
+          <t>04:38:41</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03:45:24</t>
+          <t>04:38:41</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,23 +653,273 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>56</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>03:45:24</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>05:36</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D14" t="n">
         <v>111</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>05:46</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>68</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>05:54</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>76</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:04</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>86</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>93</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>06:14</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>225_HARAS DEL SUR</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>96</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>06:21</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>103</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>109</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>06:29</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>111</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>113</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -686,7 +936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,14 +954,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:45:24</t>
+          <t>Última actualización: 04:38:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -745,12 +995,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:45:24</t>
+          <t>04:38:41</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>04:45</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -759,7 +1009,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -775,18 +1025,68 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>61</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>05:34</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>109</v>
-      </c>
-      <c r="E7" t="inlineStr">
+      <c r="D8" t="n">
+        <v>56</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>93</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -803,7 +1103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -821,14 +1121,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:45:24</t>
+          <t>Última actualización: 04:38:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -862,25 +1162,100 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>05:43</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>65</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>03:45:24</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>05:44</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>119</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:08</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>90</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:32</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>114</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1315
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:38:41</t>
+          <t>Última actualización: 05:05:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>05:23</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:45:24</t>
+          <t>04:38:41</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:36</t>
+          <t>05:34</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>05:46</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>03:45:24</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:54</t>
+          <t>05:36</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>05:46</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>05:54</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -853,21 +853,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,21 +878,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:21</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -903,23 +903,173 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>82</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>04:38:41</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>06:29</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>111</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>06:30</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>85</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>06:31</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>113</v>
-      </c>
-      <c r="E23" t="inlineStr">
+      <c r="D26" t="n">
+        <v>86</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>06:44</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>99</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>101</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>115</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -936,7 +1086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -954,14 +1104,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:38:41</t>
+          <t>Última actualización: 05:05:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -1070,23 +1220,73 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>30</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>06:11</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>93</v>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="D10" t="n">
+        <v>66</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>101</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1103,7 +1303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1121,14 +1321,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:38:41</t>
+          <t>Última actualización: 05:05:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1387,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:45:24</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1201,7 +1401,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1237,25 +1437,100 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>64</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>04:38:41</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>06:32</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>114</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:33</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>88</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>115</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1316
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:05:17</t>
+          <t>Última actualización: 05:59:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -833,16 +833,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -858,16 +858,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,21 +878,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:12</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -903,21 +903,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,21 +928,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:38:41</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:21</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,21 +953,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:27</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>04:38:41</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:29</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1003,21 +1003,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>06:44</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1033,16 +1033,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:46</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,23 +1053,473 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>06:32</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>33</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>06:44</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>45</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>05:05:17</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>101</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>48</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D29" t="n">
-        <v>115</v>
-      </c>
-      <c r="E29" t="inlineStr">
+      <c r="D33" t="n">
+        <v>61</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>66</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>66</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>07:07</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>68</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>07:12</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>73</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>77</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>82</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>07:23</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>84</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>93</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>93</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>93</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>98</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>07:39</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>100</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>07:48</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>109</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>07:52</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>113</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1086,7 +1536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1104,14 +1554,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:05:17</t>
+          <t>Última actualización: 05:59:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -1270,23 +1720,123 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:12</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>13</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>05:05:17</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>06:46</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>101</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>48</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>07:12</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>73</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07:52</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>113</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1303,7 +1853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1321,14 +1871,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:05:17</t>
+          <t>Última actualización: 05:59:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1987,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1451,7 +2001,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1487,7 +2037,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1501,7 +2051,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1512,7 +2062,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1526,9 +2076,34 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>96</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1317
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:59:00</t>
+          <t>Última actualización: 06:50:53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 64</t>
         </is>
       </c>
     </row>
@@ -1153,21 +1153,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,21 +1178,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1208,16 +1208,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,21 +1228,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1253,21 +1253,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:12</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1283,16 +1283,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,21 +1303,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1328,21 +1328,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1358,16 +1358,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,21 +1378,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1408,16 +1408,16 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:12</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,21 +1428,21 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:13</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,21 +1453,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1483,16 +1483,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1503,23 +1503,573 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>07:20</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>30</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>05:59:00</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>82</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>07:22</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>32</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>07:23</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>84</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>37</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>07:31</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>41</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>42</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>93</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>93</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>46</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>98</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>07:39</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>100</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>07:47</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>57</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>07:48</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>109</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>61</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
         <is>
           <t>07:52</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>215D_EL PATO</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D62" t="n">
         <v>113</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>73</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>82</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>08:20</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>90</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>92</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>93</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>97</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>112</v>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1536,7 +2086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1554,14 +2104,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:59:00</t>
+          <t>Última actualización: 06:50:53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -1795,21 +2345,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>07:12</t>
+          <t>06:50</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1820,23 +2370,123 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>05:59:00</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>07:12</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>73</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>61</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>07:52</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>215D_EL PATO</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D18" t="n">
         <v>113</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>93</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1853,7 +2503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1871,14 +2521,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:59:00</t>
+          <t>Última actualización: 06:50:53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -2062,12 +2712,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2076,7 +2726,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2092,18 +2742,93 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>61</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>07:35</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>96</v>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D14" t="n">
+        <v>45</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:08</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>78</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>105</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1318
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:50:53</t>
+          <t>Última actualización: 07:35:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 64</t>
+          <t>Total filas: 84</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,12 +1753,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1767,7 +1767,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,21 +1778,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,21 +1803,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,12 +1828,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:48</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,12 +1878,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>07:52</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,21 +1903,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>07:52</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1958,16 +1958,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>08:20</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,21 +1978,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:04</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,21 +2003,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2028,21 +2028,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,23 +2053,523 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>37</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>38</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
           <t>06:50:53</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>08:20</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>90</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>46</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>92</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>48</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>48</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>52</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>60</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
         <is>
           <t>08:42</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C78" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D69" t="n">
+      <c r="D78" t="n">
         <v>112</v>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>69</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>79</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>82</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>87</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>09:11</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>96</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>102</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>106</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>108</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>09:24</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>109</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>117</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>118</v>
+      </c>
+      <c r="E89" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2081,6 +2581,448 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 02/02/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 07:35:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 15</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>03:45:24</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>61</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>56</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>30</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>66</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:12</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>13</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>101</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>48</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:50</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>07:12</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>73</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>61</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>07:52</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>17</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>48</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>87</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2097,14 +3039,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 02/02/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 02/02/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:50:53</t>
+          <t>Última actualización: 07:35:06</t>
         </is>
       </c>
     </row>
@@ -2150,45 +3092,45 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:45:24</t>
+          <t>05:05:17</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:46</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2200,70 +3142,70 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>06:08</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>06:09</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>04:38:41</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:32</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
@@ -2275,45 +3217,45 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:12</t>
+          <t>06:33</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:05:17</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:46</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2325,20 +3267,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:47</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2350,487 +3292,145 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:40</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:12</t>
+          <t>08:08</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:52</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>09:09</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215D_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 02/02/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 06:50:53</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 11</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>04:38:41</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>05:43</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>65</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>05:05:17</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>05:44</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>39</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>04:38:41</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>06:08</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>90</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>06:09</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>04:38:41</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>06:32</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>114</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
           <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>06:33</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>34</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>06:59</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>9</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>07:00</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>61</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>07:35</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>45</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>08:08</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>78</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>08:35</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>105</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1319
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:35:06</t>
+          <t>Última actualización: 08:22:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 84</t>
+          <t>Total filas: 102</t>
         </is>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1288,11 +1288,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1313,11 +1313,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,7 +1753,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1763,11 +1763,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,12 +2178,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2233,16 +2233,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,21 +2253,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>08:24</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,21 +2278,21 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:27</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,21 +2303,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:33</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,21 +2328,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:34</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2358,16 +2358,16 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2378,21 +2378,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2403,21 +2403,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2433,16 +2433,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,21 +2453,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2483,16 +2483,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2503,21 +2503,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>09:24</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2533,16 +2533,16 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,23 +2553,473 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>41</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>09:04</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>42</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>48</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
           <t>07:35:06</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>09:11</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>96</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>54</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>102</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>59</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>60</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>60</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>108</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>61</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>09:24</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>109</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>70</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
         <is>
           <t>09:33</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="C102" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D89" t="n">
-        <v>118</v>
-      </c>
-      <c r="E89" t="inlineStr">
+      <c r="D102" t="n">
+        <v>71</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>09:34</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>72</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>79</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>81</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>108</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>110</v>
+      </c>
+      <c r="E107" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2586,7 +3036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2604,14 +3054,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:35:06</t>
+          <t>Última actualización: 08:22:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -2970,7 +3420,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2984,7 +3434,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2995,23 +3445,73 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>39</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>07:35:06</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>09:02</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>87</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>79</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3028,7 +3528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3046,14 +3546,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:35:06</t>
+          <t>Última actualización: 08:22:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -3412,25 +3912,100 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:36</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>14</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>46</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>07:35:06</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>09:09</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D21" t="n">
         <v>94</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>100</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1320
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:22:49</t>
+          <t>Última actualización: 08:54:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 102</t>
+          <t>Total filas: 114</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,7 +2178,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2188,11 +2188,11 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2478,21 +2478,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2503,21 +2503,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2528,12 +2528,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,21 +2553,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2578,21 +2578,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>09:04</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2603,21 +2603,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2628,12 +2628,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2653,21 +2653,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2678,21 +2678,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2708,16 +2708,16 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2728,21 +2728,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2753,21 +2753,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2778,12 +2778,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2792,7 +2792,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2808,16 +2808,16 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2833,16 +2833,16 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>09:24</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,21 +2853,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,21 +2878,21 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,21 +2903,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>09:34</t>
+          <t>09:24</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,21 +2928,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2953,21 +2953,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2978,21 +2978,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3008,18 +3008,318 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
+          <t>09:34</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>72</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>79</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>48</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>49</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>58</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>76</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
           <t>10:12</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr">
+      <c r="C113" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D107" t="n">
+      <c r="D113" t="n">
         <v>110</v>
       </c>
-      <c r="E107" t="inlineStr">
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>87</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>88</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>88</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>92</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>108</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>109</v>
+      </c>
+      <c r="E119" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3036,7 +3336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3054,14 +3354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:22:49</t>
+          <t>Última actualización: 08:54:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -3445,7 +3745,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3459,7 +3759,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3512,6 +3812,56 @@
         <v>79</v>
       </c>
       <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>48</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>92</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3528,7 +3878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3546,14 +3896,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:22:49</t>
+          <t>Última actualización: 08:54:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -3987,23 +4337,73 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:11</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>17</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>08:22:49</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>10:02</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D23" t="n">
         <v>100</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>69</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1321
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:54:22</t>
+          <t>Última actualización: 09:35:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 114</t>
+          <t>Total filas: 130</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,7 +2178,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2188,11 +2188,11 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D101" t="n">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2978,7 +2978,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2988,11 +2988,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,7 +3003,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3013,11 +3013,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3028,21 +3028,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:36</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3053,12 +3053,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3067,7 +3067,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3083,16 +3083,16 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,21 +3103,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,21 +3128,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,21 +3153,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,21 +3178,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>10:03</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,21 +3203,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>10:04</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3228,21 +3228,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3253,21 +3253,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>10:26</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3278,21 +3278,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,23 +3303,423 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>46</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
           <t>08:54:22</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr">
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>88</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>47</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>10:23</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>48</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>51</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>10:33</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>58</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>59</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>10:41</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>66</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>108</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
         <is>
           <t>10:43</t>
         </is>
       </c>
-      <c r="C119" t="inlineStr">
+      <c r="C128" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D119" t="n">
-        <v>109</v>
-      </c>
-      <c r="E119" t="inlineStr">
+      <c r="D128" t="n">
+        <v>68</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>81</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>86</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>91</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>104</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>106</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>11:27</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>112</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>11:32</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>117</v>
+      </c>
+      <c r="E135" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3336,7 +3736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3354,14 +3754,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:54:22</t>
+          <t>Última actualización: 09:35:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -3795,7 +4195,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3809,7 +4209,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -3845,7 +4245,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3859,9 +4259,34 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>86</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3878,7 +4303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3896,14 +4321,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:54:22</t>
+          <t>Última actualización: 09:35:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -4362,7 +4787,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4376,7 +4801,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -4406,6 +4831,56 @@
       <c r="E24" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>79</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11:13</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>98</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1322
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:35:44</t>
+          <t>Última actualización: 10:45:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 130</t>
+          <t>Total filas: 153</t>
         </is>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1288,11 +1288,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1313,11 +1313,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -3328,7 +3328,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3338,11 +3338,11 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,7 +3353,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3363,11 +3363,11 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3553,21 +3553,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>10:56</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3578,21 +3578,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:46</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3603,21 +3603,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>10:52</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,21 +3628,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>10:53</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,21 +3653,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>10:56</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,21 +3678,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,23 +3703,598 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
+          <t>11:03</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>18</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>19</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>21</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>11:11</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>26</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>11:12</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>27</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>34</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>36</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>11:27</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>42</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
           <t>11:32</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr">
+      <c r="C143" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D135" t="n">
-        <v>117</v>
-      </c>
-      <c r="E135" t="inlineStr">
+      <c r="D143" t="n">
+        <v>47</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>11:34</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>49</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>11:35</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>50</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>56</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>11:43</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>58</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>66</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>11:59</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>74</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>77</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>81</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>81</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>12:16</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>91</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>95</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>95</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>96</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>111</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>113</v>
+      </c>
+      <c r="E158" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3736,7 +4311,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3754,14 +4329,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:35:44</t>
+          <t>Última actualización: 10:45:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -4270,7 +4845,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4284,9 +4859,59 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>66</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>95</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4303,7 +4928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4321,14 +4946,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:35:44</t>
+          <t>Última actualización: 10:45:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -4837,7 +5462,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4851,7 +5476,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -4862,7 +5487,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4876,11 +5501,36 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>79</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1323
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E158"/>
+  <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:45:47</t>
+          <t>Última actualización: 11:27:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 153</t>
+          <t>Total filas: 165</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,7 +1753,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1763,11 +1763,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,7 +2178,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2188,11 +2188,11 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2978,7 +2978,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2988,11 +2988,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,7 +3003,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3013,11 +3013,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,21 +3903,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>11:28</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,21 +3928,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>11:34</t>
+          <t>11:32</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,21 +3953,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>11:35</t>
+          <t>11:34</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3978,21 +3978,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,21 +4003,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>11:43</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,21 +4028,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:43</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,21 +4053,21 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,21 +4078,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>12:02</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4103,21 +4103,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,21 +4128,21 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:02</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,21 +4153,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,21 +4178,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4203,12 +4203,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4217,7 +4217,7 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4233,16 +4233,16 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4278,23 +4278,323 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>53</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>54</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>55</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>69</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
           <t>12:38</t>
         </is>
       </c>
-      <c r="C158" t="inlineStr">
+      <c r="C162" t="inlineStr">
         <is>
           <t>17_179 Y 38</t>
         </is>
       </c>
-      <c r="D158" t="n">
-        <v>113</v>
-      </c>
-      <c r="E158" t="inlineStr">
+      <c r="D162" t="n">
+        <v>71</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>74</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>81</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>83</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>12:58</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>91</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>99</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>106</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>114</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>13:22</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>115</v>
+      </c>
+      <c r="E170" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4311,7 +4611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4329,14 +4629,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:45:47</t>
+          <t>Última actualización: 11:27:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -4870,7 +5170,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4884,7 +5184,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4895,7 +5195,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4909,9 +5209,34 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>106</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4928,7 +5253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4946,14 +5271,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:45:47</t>
+          <t>Última actualización: 11:27:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -5512,7 +5837,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5526,11 +5851,36 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>12:53</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>86</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1324
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E170"/>
+  <dimension ref="A1:E188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:27:45</t>
+          <t>Última actualización: 12:06:53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 165</t>
+          <t>Total filas: 183</t>
         </is>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1288,11 +1288,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1313,11 +1313,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,7 +1678,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1688,11 +1688,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,7 +1753,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1763,11 +1763,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -3328,7 +3328,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3338,11 +3338,11 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,7 +3353,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3363,11 +3363,11 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4203,7 +4203,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4213,11 +4213,11 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,21 +4228,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>10:45:47</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>10:45:47</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4278,7 +4278,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4288,11 +4288,11 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4303,21 +4303,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,21 +4328,21 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4358,16 +4358,16 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,21 +4378,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4408,7 +4408,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -4417,7 +4417,7 @@
         </is>
       </c>
       <c r="D163" t="n">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,12 +4428,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -4442,7 +4442,7 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,21 +4453,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4478,21 +4478,21 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>12:58</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,21 +4503,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,21 +4528,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4558,16 +4558,16 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,23 +4578,473 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>42</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>44</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>49</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
           <t>11:27:45</t>
         </is>
       </c>
-      <c r="B170" t="inlineStr">
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>12:58</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>91</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>56</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>60</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>61</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>67</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>74</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>114</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
         <is>
           <t>13:22</t>
         </is>
       </c>
-      <c r="C170" t="inlineStr">
+      <c r="C180" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D170" t="n">
+      <c r="D180" t="n">
         <v>115</v>
       </c>
-      <c r="E170" t="inlineStr">
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>79</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>80</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>13:34</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>88</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>13:37</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>91</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>100</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>104</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>109</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>110</v>
+      </c>
+      <c r="E188" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4611,7 +5061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4629,14 +5079,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:27:45</t>
+          <t>Última actualización: 12:06:53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -5195,7 +5645,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5209,7 +5659,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -5220,7 +5670,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -5234,9 +5684,34 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>104</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5253,7 +5728,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5271,14 +5746,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:27:45</t>
+          <t>Última actualización: 12:06:53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -5862,25 +6337,75 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>12:53</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>86</v>
-      </c>
-      <c r="E28" t="inlineStr">
+      <c r="D29" t="n">
+        <v>47</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>84</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1325
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E188"/>
+  <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:06:53</t>
+          <t>Última actualización: 12:48:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 183</t>
+          <t>Total filas: 195</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,7 +1678,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1688,11 +1688,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D100" t="n">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -2978,7 +2978,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2988,11 +2988,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,7 +3003,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3013,11 +3013,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4608,16 +4608,16 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,21 +4628,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>12:55</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,21 +4653,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>12:58</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>91</v>
+        <v>2</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,21 +4678,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:51</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,21 +4703,21 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,21 +4728,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>12:58</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,21 +4753,21 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,21 +4778,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,21 +4803,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4828,12 +4828,12 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>13:22</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -4842,7 +4842,7 @@
         </is>
       </c>
       <c r="D180" t="n">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4853,21 +4853,21 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,21 +4878,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4903,21 +4903,21 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>13:34</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4928,21 +4928,21 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>13:37</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,21 +4953,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:22</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4983,16 +4983,16 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,21 +5003,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>13:55</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,23 +5028,323 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>39</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>43</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>13:34</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>46</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
           <t>12:06:53</t>
         </is>
       </c>
-      <c r="B188" t="inlineStr">
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>13:37</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>91</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>58</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>62</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>67</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
         <is>
           <t>13:56</t>
         </is>
       </c>
-      <c r="C188" t="inlineStr">
+      <c r="C195" t="inlineStr">
         <is>
           <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
-      <c r="D188" t="n">
-        <v>110</v>
-      </c>
-      <c r="E188" t="inlineStr">
+      <c r="D195" t="n">
+        <v>68</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>76</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>88</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>91</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>92</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>116</v>
+      </c>
+      <c r="E200" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5056,673 +5356,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215 - 02/02/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 12:06:53</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 24</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>04:38:41</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>04:45</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>7</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>03:45:24</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>04:46</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>61</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>04:38:41</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>05:34</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>56</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>05:05:17</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>05:35</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>30</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>05:05:17</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>06:11</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>66</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>06:12</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>13</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>05:05:17</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>06:46</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>101</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>06:47</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>48</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>06:50</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>07:11</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>21</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>07:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>73</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>07:51</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>61</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>07:35:06</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>07:52</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>17</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>08:22:49</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>08:23</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>08:54:22</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>09:01</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>7</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>07:35:06</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>09:02</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>87</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>09:35:44</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>09:41</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>6</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>08:54:22</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>09:42</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>48</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>09:35:44</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>10:26</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>51</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>10:45:47</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>11:01</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>16</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>11:27:45</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>11:51</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>24</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>12:06:53</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>12:20</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>14</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>12:06:53</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>13:13</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>67</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>12:06:53</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>13:50</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>104</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5739,14 +5372,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 02/02/2026</t>
+          <t>LÍNEA 141 - LP1912-215 - 02/02/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:06:53</t>
+          <t>Última actualización: 12:48:55</t>
         </is>
       </c>
     </row>
@@ -5792,6 +5425,698 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>03:45:24</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>61</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>56</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>30</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>66</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:12</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>13</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>101</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>48</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:50</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>07:12</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>73</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>61</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>07:52</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>17</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>7</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>87</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>48</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>51</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>16</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>24</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>14</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>25</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>62</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>91</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173 - 02/02/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 12:48:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 27</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>05:43</t>
         </is>
       </c>
@@ -6387,23 +6712,73 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>6</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>13:30</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D30" t="n">
-        <v>84</v>
-      </c>
-      <c r="E30" t="inlineStr">
+      <c r="D31" t="n">
+        <v>42</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:08</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>80</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1326
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E200"/>
+  <dimension ref="A1:E216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:48:55</t>
+          <t>Última actualización: 13:18:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 195</t>
+          <t>Total filas: 211</t>
         </is>
       </c>
     </row>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,7 +2178,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2188,11 +2188,11 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -3328,7 +3328,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3338,11 +3338,11 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,7 +3353,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3363,11 +3363,11 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -4588,7 +4588,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4903,21 +4903,21 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4928,21 +4928,21 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,21 +4953,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>13:22</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4978,21 +4978,21 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,21 +5003,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:22</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,12 +5028,12 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>13:27</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -5042,7 +5042,7 @@
         </is>
       </c>
       <c r="D188" t="n">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5053,21 +5053,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>13:31</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5078,21 +5078,21 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>13:34</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5103,21 +5103,21 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>13:37</t>
+          <t>13:27</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5128,21 +5128,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:28</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5158,16 +5158,16 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:31</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,21 +5178,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>13:55</t>
+          <t>13:34</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,21 +5203,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,12 +5228,12 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:37</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -5242,7 +5242,7 @@
         </is>
       </c>
       <c r="D196" t="n">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5253,21 +5253,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5278,21 +5278,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>14:19</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,21 +5303,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5333,18 +5333,418 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>67</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>38</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>38</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>46</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>46</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>58</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>91</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>62</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>92</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>63</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
           <t>14:44</t>
         </is>
       </c>
-      <c r="C200" t="inlineStr">
+      <c r="C210" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D200" t="n">
+      <c r="D210" t="n">
         <v>116</v>
       </c>
-      <c r="E200" t="inlineStr">
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>87</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>98</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>100</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>102</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>107</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>115</v>
+      </c>
+      <c r="E216" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5356,698 +5756,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215 - 02/02/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 12:48:55</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 25</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>04:38:41</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>04:45</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>7</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>03:45:24</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>04:46</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>61</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>04:38:41</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>05:34</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>56</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>05:05:17</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>05:35</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>30</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>05:05:17</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>06:11</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>66</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>06:12</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>13</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>05:05:17</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>06:46</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>101</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>06:47</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>48</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>06:50</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>07:11</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>21</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>05:59:00</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>07:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>73</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>06:50:53</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>07:51</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>61</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>07:35:06</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>07:52</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>17</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>08:22:49</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>08:23</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>08:54:22</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>09:01</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>7</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>07:35:06</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>09:02</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>87</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>09:35:44</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>09:41</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>6</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>08:54:22</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>09:42</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>48</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>09:35:44</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>10:26</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>51</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>10:45:47</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>11:01</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>16</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>11:27:45</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>11:51</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>24</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>12:06:53</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>12:20</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>14</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>12:48:55</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>13:13</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>25</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>12:48:55</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>13:50</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>62</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>12:48:55</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>14:19</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>91</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6064,14 +5772,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 02/02/2026</t>
+          <t>LÍNEA 141 - LP1912-215 - 02/02/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:48:55</t>
+          <t>Última actualización: 13:18:34</t>
         </is>
       </c>
     </row>
@@ -6117,6 +5825,748 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>03:45:24</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>61</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>56</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>30</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>66</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:12</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>13</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>05:05:17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>101</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>48</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:50</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>05:59:00</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>07:12</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>73</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>06:50:53</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>61</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>07:52</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>17</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08:22:49</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>7</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>07:35:06</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>87</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>08:54:22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>48</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>09:35:44</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>51</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:45:47</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>16</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>11:27:45</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>24</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>12:06:53</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>14</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>25</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>32</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>91</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>62</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>100</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173 - 02/02/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 13:18:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04:38:41</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>05:43</t>
         </is>
       </c>
@@ -6762,25 +7212,100 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>13</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>12:48:55</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>14:08</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="D33" t="n">
         <v>80</v>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>51</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>13:18:34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>95</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1327
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:18:34</t>
+          <t>Última actualización: 14:04:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 211</t>
+          <t>Total filas: 228</t>
         </is>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1288,11 +1288,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1313,11 +1313,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2978,7 +2978,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2988,11 +2988,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,7 +3003,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3013,11 +3013,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4228,7 +4228,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4238,11 +4238,11 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D201" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5413,7 +5413,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -5428,7 +5428,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -5438,11 +5438,11 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5453,21 +5453,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5478,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>14:19</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,21 +5528,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:07</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,21 +5553,21 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:12</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5578,21 +5578,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,21 +5603,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,21 +5628,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:19</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,21 +5653,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,21 +5703,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>107</v>
+        <v>17</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,23 +5728,448 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>40</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
           <t>13:18:34</t>
         </is>
       </c>
-      <c r="B216" t="inlineStr">
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>87</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>52</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>54</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>56</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>61</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>15:10</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>66</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
         <is>
           <t>15:13</t>
         </is>
       </c>
-      <c r="C216" t="inlineStr">
+      <c r="C223" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D216" t="n">
-        <v>115</v>
-      </c>
-      <c r="E216" t="inlineStr">
+      <c r="D223" t="n">
+        <v>69</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>76</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>77</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>88</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>93</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>94</v>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>94</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>102</v>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>15:50</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>106</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>110</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>113</v>
+      </c>
+      <c r="E233" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5761,7 +6186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5779,14 +6204,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:18:34</t>
+          <t>Última actualización: 14:04:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -6445,7 +6870,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -6459,7 +6884,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -6470,7 +6895,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -6484,9 +6909,34 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>94</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6503,7 +6953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6521,14 +6971,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:18:34</t>
+          <t>Última actualización: 14:04:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -7287,25 +7737,75 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>14:11</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>7</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>14:53</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D35" t="n">
-        <v>95</v>
-      </c>
-      <c r="E35" t="inlineStr">
+      <c r="D36" t="n">
+        <v>49</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>90</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1328
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:04:21</t>
+          <t>Última actualización: 14:52:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 228</t>
+          <t>Total filas: 244</t>
         </is>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1678,7 +1678,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1688,11 +1688,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,7 +2178,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2188,11 +2188,11 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -3328,7 +3328,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3338,11 +3338,11 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,7 +3353,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3363,11 +3363,11 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4228,7 +4228,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4238,11 +4238,11 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5403,7 +5403,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -5413,11 +5413,11 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5428,7 +5428,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -5438,11 +5438,11 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5463,7 +5463,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D205" t="n">
@@ -5488,7 +5488,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D206" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5778,21 +5778,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5808,16 +5808,16 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5828,21 +5828,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:57</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5853,21 +5853,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5878,21 +5878,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5903,21 +5903,21 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,21 +5928,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,21 +5953,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5983,16 +5983,16 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6003,21 +6003,21 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:14</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6028,21 +6028,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,21 +6053,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>15:50</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>15:37</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6158,18 +6158,418 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>94</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>94</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>47</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>54</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>102</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>15:47</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>55</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>14:04:21</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>15:50</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>106</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>62</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>64</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
           <t>15:57</t>
         </is>
       </c>
-      <c r="C233" t="inlineStr">
+      <c r="C242" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D233" t="n">
-        <v>113</v>
-      </c>
-      <c r="E233" t="inlineStr">
+      <c r="D242" t="n">
+        <v>65</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>83</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>88</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>97</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>98</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>101</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>111</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>111</v>
+      </c>
+      <c r="E249" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6186,7 +6586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6204,14 +6604,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:04:21</t>
+          <t>Última actualización: 14:52:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -6895,7 +7295,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -6909,7 +7309,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -6937,6 +7337,56 @@
         <v>94</v>
       </c>
       <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>47</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>88</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6953,7 +7403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6971,14 +7421,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:04:21</t>
+          <t>Última actualización: 14:52:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -7762,7 +8212,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -7776,7 +8226,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -7787,7 +8237,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>14:52:16</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7801,11 +8251,36 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>82</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1329
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-02.xlsx
+++ b/data/horarios-141-2026-02-02.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E249"/>
+  <dimension ref="A1:E262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:52:16</t>
+          <t>Última actualización: 15:30:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 244</t>
+          <t>Total filas: 257</t>
         </is>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1288,11 +1288,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1313,11 +1313,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:59:00</t>
+          <t>06:50:53</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,7 +1678,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>06:50:53</t>
+          <t>05:59:00</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1688,11 +1688,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>07:35:06</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>07:35:06</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2978,7 +2978,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>08:22:49</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2988,11 +2988,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,7 +3003,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:22:49</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3013,11 +3013,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3328,7 +3328,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>08:54:22</t>
+          <t>09:35:44</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3338,11 +3338,11 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,7 +3353,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>09:35:44</t>
+          <t>08:54:22</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3363,11 +3363,11 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>11:27:45</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4228,7 +4228,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>11:27:45</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4238,11 +4238,11 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:06:53</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4613,7 +4613,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>12:06:53</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5403,7 +5403,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>13:18:34</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -5413,11 +5413,11 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5428,7 +5428,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>13:18:34</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -5438,11 +5438,11 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5488,7 +5488,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D206" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>12:48:55</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:48:55</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:31</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:31</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6178,21 +6178,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:37</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,12 +6203,12 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>15:39</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -6217,7 +6217,7 @@
         </is>
       </c>
       <c r="D235" t="n">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6228,21 +6228,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6253,21 +6253,21 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:39</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>102</v>
+        <v>9</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6278,12 +6278,12 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>15:46</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -6292,7 +6292,7 @@
         </is>
       </c>
       <c r="D238" t="n">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,12 +6303,12 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>14:04:21</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>15:50</t>
+          <t>15:46</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -6317,7 +6317,7 @@
         </is>
       </c>
       <c r="D239" t="n">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,21 +6328,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>15:47</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,21 +6353,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>14:04:21</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:50</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,21 +6378,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:54</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,21 +6403,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,21 +6428,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,21 +6453,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6478,21 +6478,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6503,21 +6503,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6528,21 +6528,21 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6553,23 +6553,348 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>51</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
           <t>14:52:16</t>
         </is>
       </c>
-      <c r="B249" t="inlineStr">
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>97</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>98</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>14:52:16</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>101</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>70</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
         <is>
           <t>16:43</t>
         </is>
       </c>
-      <c r="C249" t="inlineStr">
+      <c r="C254" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D249" t="n">
+      <c r="D254" t="n">
+        <v>73</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>73</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>86</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>88</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>95</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>95</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
         <v>111</v>
       </c>
-      <c r="E249" t="inlineStr">
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>114</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>118</v>
+      </c>
+      <c r="E262" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6586,7 +6911,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6604,14 +6929,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:52:16</t>
+          <t>Última actualización: 15:30:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
     </row>
@@ -7345,7 +7670,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -7359,7 +7684,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -7370,7 +7695,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -7384,9 +7709,34 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>95</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7403,7 +7753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7421,14 +7771,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:52:16</t>
+          <t>Última actualización: 15:30:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
     </row>
@@ -8237,7 +8587,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -8251,7 +8601,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -8262,7 +8612,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>14:52:16</t>
+          <t>15:30:15</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -8276,11 +8626,61 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>83</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>15:30:15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>17:14</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>104</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>